<commit_message>
Code to create a summary of the results of the overall training process
</commit_message>
<xml_diff>
--- a/fine_tuning/training_summary_acl_sentiment.xlsx
+++ b/fine_tuning/training_summary_acl_sentiment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="74">
   <si>
     <t>training_lang</t>
   </si>
@@ -139,28 +139,28 @@
     <t>1:08:33</t>
   </si>
   <si>
-    <t>0:20:01</t>
+    <t>0:45:25</t>
   </si>
   <si>
     <t>0:16:46</t>
   </si>
   <si>
+    <t>0:40:37</t>
+  </si>
+  <si>
     <t>0:29:42</t>
   </si>
   <si>
-    <t>0:40:37</t>
+    <t>0:17:57</t>
   </si>
   <si>
     <t>0:07:58</t>
   </si>
   <si>
-    <t>0:17:57</t>
-  </si>
-  <si>
-    <t>0:05:40</t>
-  </si>
-  <si>
-    <t>0:15:33</t>
+    <t>0:12:08</t>
+  </si>
+  <si>
+    <t>0:12:09</t>
   </si>
   <si>
     <t>3:38:59</t>
@@ -172,7 +172,7 @@
     <t>0:23:47</t>
   </si>
   <si>
-    <t>0:16:16</t>
+    <t>2:10:39</t>
   </si>
   <si>
     <t>1:06:01</t>
@@ -181,25 +181,28 @@
     <t>0:42:23</t>
   </si>
   <si>
-    <t>3:29:13</t>
-  </si>
-  <si>
-    <t>0:09:47</t>
-  </si>
-  <si>
-    <t>0:16:09</t>
+    <t>3:38:33</t>
+  </si>
+  <si>
+    <t>4:04:22</t>
+  </si>
+  <si>
+    <t>0:20:22</t>
+  </si>
+  <si>
+    <t>0:34:10</t>
+  </si>
+  <si>
+    <t>0:19:15</t>
   </si>
   <si>
     <t>0:52:43</t>
   </si>
   <si>
-    <t>0:15:52</t>
-  </si>
-  <si>
-    <t>0:14:57</t>
-  </si>
-  <si>
-    <t>0:31:09</t>
+    <t>0:14:52</t>
+  </si>
+  <si>
+    <t>0:32:51</t>
   </si>
   <si>
     <t>1:38:24</t>
@@ -208,13 +211,13 @@
     <t>2:27:00</t>
   </si>
   <si>
-    <t>0:03:51</t>
-  </si>
-  <si>
-    <t>0:11:46</t>
-  </si>
-  <si>
-    <t>4:36:24</t>
+    <t>0:21:10</t>
+  </si>
+  <si>
+    <t>1:30:33</t>
+  </si>
+  <si>
+    <t>2:14:46</t>
   </si>
   <si>
     <t>2:23:47</t>
@@ -223,13 +226,13 @@
     <t>2:19:12</t>
   </si>
   <si>
-    <t>0:18:53</t>
-  </si>
-  <si>
-    <t>0:12:04</t>
-  </si>
-  <si>
-    <t>0:08:40</t>
+    <t>0:24:40</t>
+  </si>
+  <si>
+    <t>0:10:12</t>
+  </si>
+  <si>
+    <t>0:04:06</t>
   </si>
   <si>
     <t>0:23:15</t>
@@ -590,7 +593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -778,7 +781,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
@@ -787,28 +790,28 @@
         <v>256</v>
       </c>
       <c r="E4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>2E-05</v>
       </c>
       <c r="G4">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H4">
-        <v>0.8798861445999497</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>0.8458000484144276</v>
+        <v>0.8638888888888889</v>
       </c>
       <c r="J4" t="s">
         <v>41</v>
       </c>
       <c r="K4">
-        <v>0.7450980392156863</v>
+        <v>0.7777777777777779</v>
       </c>
       <c r="L4">
-        <v>0.9465020576131689</v>
+        <v>0.95</v>
       </c>
       <c r="M4">
         <v>1029</v>
@@ -829,7 +832,7 @@
         <v>23.32847424684159</v>
       </c>
       <c r="S4">
-        <v>356</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -899,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6">
         <v>256</v>
@@ -911,22 +914,22 @@
         <v>2E-05</v>
       </c>
       <c r="G6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H6">
-        <v>0.9950652044063213</v>
+        <v>0.9961744704413876</v>
       </c>
       <c r="I6">
-        <v>0.9371932107161867</v>
+        <v>0.9461951565508158</v>
       </c>
       <c r="J6" t="s">
         <v>43</v>
       </c>
       <c r="K6">
-        <v>0.8918918918918919</v>
+        <v>0.906474820143885</v>
       </c>
       <c r="L6">
-        <v>0.9824945295404814</v>
+        <v>0.9859154929577464</v>
       </c>
       <c r="M6">
         <v>3724</v>
@@ -944,7 +947,7 @@
         <v>1092</v>
       </c>
       <c r="R6">
-        <v>32.97261009667024</v>
+        <v>26.39366272824919</v>
       </c>
       <c r="S6">
         <v>3724</v>
@@ -958,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>256</v>
@@ -970,22 +973,22 @@
         <v>2E-05</v>
       </c>
       <c r="G7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>0.9961744704413876</v>
+        <v>0.9950652044063213</v>
       </c>
       <c r="I7">
-        <v>0.9461951565508158</v>
+        <v>0.9371932107161867</v>
       </c>
       <c r="J7" t="s">
         <v>44</v>
       </c>
       <c r="K7">
-        <v>0.906474820143885</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="L7">
-        <v>0.9859154929577464</v>
+        <v>0.9824945295404814</v>
       </c>
       <c r="M7">
         <v>3724</v>
@@ -1003,7 +1006,7 @@
         <v>1092</v>
       </c>
       <c r="R7">
-        <v>26.39366272824919</v>
+        <v>32.97261009667024</v>
       </c>
       <c r="S7">
         <v>3724</v>
@@ -1017,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>256</v>
@@ -1029,22 +1032,22 @@
         <v>2E-05</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>0.9036462117225303</v>
+        <v>0.9683249930298837</v>
       </c>
       <c r="I8">
-        <v>0.8284664508791881</v>
+        <v>0.729086055899936</v>
       </c>
       <c r="J8" t="s">
         <v>45</v>
       </c>
       <c r="K8">
-        <v>0.7639751552795031</v>
+        <v>0.6246056782334385</v>
       </c>
       <c r="L8">
-        <v>0.8929577464788733</v>
+        <v>0.8335664335664336</v>
       </c>
       <c r="M8">
         <v>2675</v>
@@ -1062,7 +1065,7 @@
         <v>1818</v>
       </c>
       <c r="R8">
-        <v>28.4381308411215</v>
+        <v>29.66728971962617</v>
       </c>
       <c r="S8">
         <v>2675</v>
@@ -1076,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9">
         <v>256</v>
@@ -1088,22 +1091,22 @@
         <v>2E-05</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>0.9683249930298837</v>
+        <v>0.9036462117225303</v>
       </c>
       <c r="I9">
-        <v>0.729086055899936</v>
+        <v>0.8284664508791881</v>
       </c>
       <c r="J9" t="s">
         <v>46</v>
       </c>
       <c r="K9">
-        <v>0.6246056782334385</v>
+        <v>0.7639751552795031</v>
       </c>
       <c r="L9">
-        <v>0.8335664335664336</v>
+        <v>0.8929577464788733</v>
       </c>
       <c r="M9">
         <v>2675</v>
@@ -1121,7 +1124,7 @@
         <v>1818</v>
       </c>
       <c r="R9">
-        <v>29.66728971962617</v>
+        <v>28.4381308411215</v>
       </c>
       <c r="S9">
         <v>2675</v>
@@ -1141,28 +1144,28 @@
         <v>256</v>
       </c>
       <c r="E10">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <v>2E-05</v>
       </c>
       <c r="G10">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H10">
-        <v>0.9657484192800178</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>0.7426900584795322</v>
+        <v>0.9288793103448276</v>
       </c>
       <c r="J10" t="s">
         <v>47</v>
       </c>
       <c r="K10">
-        <v>0.9298245614035087</v>
+        <v>0.9827586206896551</v>
       </c>
       <c r="L10">
-        <v>0.5555555555555556</v>
+        <v>0.875</v>
       </c>
       <c r="M10">
         <v>462</v>
@@ -1197,31 +1200,31 @@
         <v>38</v>
       </c>
       <c r="D11">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E11">
         <v>16</v>
       </c>
       <c r="F11">
-        <v>2E-05</v>
+        <v>2E-06</v>
       </c>
       <c r="G11">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H11">
-        <v>0.9611389157589267</v>
+        <v>0.969041769041769</v>
       </c>
       <c r="I11">
-        <v>0.7642857142857142</v>
+        <v>0.9200968523002421</v>
       </c>
       <c r="J11" t="s">
         <v>48</v>
       </c>
       <c r="K11">
-        <v>0.9285714285714286</v>
+        <v>0.9830508474576271</v>
       </c>
       <c r="L11">
-        <v>0.6</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="M11">
         <v>462</v>
@@ -1436,28 +1439,28 @@
         <v>256</v>
       </c>
       <c r="E15">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F15">
         <v>2E-05</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="H15">
-        <v>0.9869630028916674</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>0.8460960960960962</v>
+        <v>0.8533914403844005</v>
       </c>
       <c r="J15" t="s">
         <v>52</v>
       </c>
       <c r="K15">
-        <v>0.861111111111111</v>
+        <v>0.8596491228070176</v>
       </c>
       <c r="L15">
-        <v>0.8310810810810811</v>
+        <v>0.8471337579617835</v>
       </c>
       <c r="M15">
         <v>2384</v>
@@ -1619,22 +1622,22 @@
         <v>2E-05</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H18">
-        <v>0.9782159712373002</v>
+        <v>0.9742329080543712</v>
       </c>
       <c r="I18">
-        <v>0.9239197941620086</v>
+        <v>0.925558022671497</v>
       </c>
       <c r="J18" t="s">
         <v>55</v>
       </c>
       <c r="K18">
-        <v>0.8717948717948717</v>
+        <v>0.8743718592964823</v>
       </c>
       <c r="L18">
-        <v>0.9760447165291456</v>
+        <v>0.9767441860465116</v>
       </c>
       <c r="M18">
         <v>31217</v>
@@ -1660,7 +1663,7 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -1678,43 +1681,43 @@
         <v>2E-05</v>
       </c>
       <c r="G19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H19">
-        <v>0.9932997546170735</v>
+        <v>0.9833652821029948</v>
       </c>
       <c r="I19">
-        <v>0.8925831202046035</v>
+        <v>0.9307842026806231</v>
       </c>
       <c r="J19" t="s">
         <v>56</v>
       </c>
       <c r="K19">
-        <v>0.8431372549019608</v>
+        <v>0.881949733434882</v>
       </c>
       <c r="L19">
-        <v>0.9420289855072463</v>
+        <v>0.9796186719263642</v>
       </c>
       <c r="M19">
-        <v>1355</v>
+        <v>31217</v>
       </c>
       <c r="N19">
-        <v>0.7158671586715867</v>
+        <v>0.8503059230547458</v>
       </c>
       <c r="O19">
-        <v>1.789325842696629</v>
+        <v>3.340038519152579</v>
       </c>
       <c r="P19">
-        <v>0.6938997821350763</v>
+        <v>0.5880269750970124</v>
       </c>
       <c r="Q19">
-        <v>770</v>
+        <v>9346</v>
       </c>
       <c r="R19">
-        <v>80.20959409594096</v>
+        <v>138.3485600794439</v>
       </c>
       <c r="S19">
-        <v>1355</v>
+        <v>31217</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -1731,28 +1734,28 @@
         <v>256</v>
       </c>
       <c r="E20">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F20">
         <v>2E-05</v>
       </c>
       <c r="G20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H20">
-        <v>0.9980541835054633</v>
+        <v>0.9951478755388181</v>
       </c>
       <c r="I20">
-        <v>0.8154761904761905</v>
+        <v>0.8207885304659498</v>
       </c>
       <c r="J20" t="s">
         <v>57</v>
       </c>
       <c r="K20">
-        <v>0.7142857142857143</v>
+        <v>0.7311827956989247</v>
       </c>
       <c r="L20">
-        <v>0.9166666666666667</v>
+        <v>0.9103942652329748</v>
       </c>
       <c r="M20">
         <v>1355</v>
@@ -1778,7 +1781,7 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -1790,49 +1793,49 @@
         <v>256</v>
       </c>
       <c r="E21">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F21">
         <v>2E-05</v>
       </c>
       <c r="G21">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="H21">
-        <v>0.9975678549960697</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>0.9112890563667766</v>
+        <v>0.9433623014683847</v>
       </c>
       <c r="J21" t="s">
         <v>58</v>
       </c>
       <c r="K21">
-        <v>0.8484848484848485</v>
+        <v>0.9148936170212766</v>
       </c>
       <c r="L21">
-        <v>0.9740932642487047</v>
+        <v>0.971830985915493</v>
       </c>
       <c r="M21">
-        <v>789</v>
+        <v>1355</v>
       </c>
       <c r="N21">
-        <v>0.8466413181242078</v>
+        <v>0.7158671586715867</v>
       </c>
       <c r="O21">
-        <v>3.260330578512397</v>
+        <v>1.789325842696629</v>
       </c>
       <c r="P21">
-        <v>0.5905688622754491</v>
+        <v>0.6938997821350763</v>
       </c>
       <c r="Q21">
-        <v>242</v>
+        <v>770</v>
       </c>
       <c r="R21">
-        <v>19.80481622306717</v>
+        <v>80.20959409594096</v>
       </c>
       <c r="S21">
-        <v>789</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -1849,28 +1852,28 @@
         <v>256</v>
       </c>
       <c r="E22">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F22">
         <v>2E-05</v>
       </c>
       <c r="G22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22">
-        <v>0.8403203014601979</v>
+        <v>0.8907860824742269</v>
       </c>
       <c r="J22" t="s">
         <v>59</v>
       </c>
       <c r="K22">
-        <v>0.7272727272727272</v>
+        <v>0.8125</v>
       </c>
       <c r="L22">
-        <v>0.9533678756476685</v>
+        <v>0.9690721649484536</v>
       </c>
       <c r="M22">
         <v>789</v>
@@ -1896,13 +1899,13 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D23">
         <v>256</v>
@@ -1914,43 +1917,43 @@
         <v>2E-05</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="H23">
-        <v>0.8951288469430809</v>
+        <v>0.9975678549960697</v>
       </c>
       <c r="I23">
-        <v>0.7431260813962235</v>
+        <v>0.9112890563667766</v>
       </c>
       <c r="J23" t="s">
         <v>60</v>
       </c>
       <c r="K23">
-        <v>0.7203791469194312</v>
+        <v>0.8484848484848485</v>
       </c>
       <c r="L23">
-        <v>0.7658730158730159</v>
+        <v>0.9740932642487047</v>
       </c>
       <c r="M23">
-        <v>3237</v>
+        <v>789</v>
       </c>
       <c r="N23">
-        <v>0.5817114612295335</v>
+        <v>0.8466413181242078</v>
       </c>
       <c r="O23">
-        <v>1.195347119645495</v>
+        <v>3.260330578512397</v>
       </c>
       <c r="P23">
-        <v>0.8595326606479022</v>
+        <v>0.5905688622754491</v>
       </c>
       <c r="Q23">
-        <v>2708</v>
+        <v>242</v>
       </c>
       <c r="R23">
-        <v>44.17763361136855</v>
+        <v>19.80481622306717</v>
       </c>
       <c r="S23">
-        <v>3237</v>
+        <v>789</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -1961,34 +1964,34 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24">
         <v>256</v>
       </c>
       <c r="E24">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F24">
         <v>2E-05</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>0.9266068895486292</v>
+        <v>0.9555193039907464</v>
       </c>
       <c r="I24">
-        <v>0.8074116089998109</v>
+        <v>0.7485134362492853</v>
       </c>
       <c r="J24" t="s">
         <v>61</v>
       </c>
       <c r="K24">
-        <v>0.7853658536585365</v>
+        <v>0.712121212121212</v>
       </c>
       <c r="L24">
-        <v>0.8294573643410853</v>
+        <v>0.7849056603773585</v>
       </c>
       <c r="M24">
         <v>3237</v>
@@ -2006,7 +2009,7 @@
         <v>2708</v>
       </c>
       <c r="R24">
-        <v>39.5863453815261</v>
+        <v>44.17763361136855</v>
       </c>
       <c r="S24">
         <v>3237</v>
@@ -2014,7 +2017,7 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -2026,7 +2029,7 @@
         <v>256</v>
       </c>
       <c r="E25">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F25">
         <v>2E-05</v>
@@ -2035,40 +2038,40 @@
         <v>5</v>
       </c>
       <c r="H25">
-        <v>0.9967218141513501</v>
+        <v>0.9886034057168788</v>
       </c>
       <c r="I25">
-        <v>0.9927476606484178</v>
+        <v>0.8188714171214839</v>
       </c>
       <c r="J25" t="s">
         <v>62</v>
       </c>
       <c r="K25">
-        <v>0.9924286546301689</v>
+        <v>0.7918781725888325</v>
       </c>
       <c r="L25">
-        <v>0.9930666666666667</v>
+        <v>0.8458646616541353</v>
       </c>
       <c r="M25">
-        <v>13976</v>
+        <v>3237</v>
       </c>
       <c r="N25">
-        <v>0.5</v>
+        <v>0.5817114612295335</v>
       </c>
       <c r="O25">
-        <v>1.00899723162104</v>
+        <v>1.195347119645495</v>
       </c>
       <c r="P25">
-        <v>0.9911618069194742</v>
+        <v>0.8595326606479022</v>
       </c>
       <c r="Q25">
-        <v>13976</v>
+        <v>2708</v>
       </c>
       <c r="R25">
-        <v>124.8941041785919</v>
+        <v>39.5863453815261</v>
       </c>
       <c r="S25">
-        <v>13976</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -2079,7 +2082,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D26">
         <v>256</v>
@@ -2091,22 +2094,22 @@
         <v>2E-05</v>
       </c>
       <c r="G26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H26">
-        <v>0.9968749313981738</v>
+        <v>0.9967218141513501</v>
       </c>
       <c r="I26">
-        <v>0.9823813321094111</v>
+        <v>0.9927476606484178</v>
       </c>
       <c r="J26" t="s">
         <v>63</v>
       </c>
       <c r="K26">
-        <v>0.9819770617149098</v>
+        <v>0.9924286546301689</v>
       </c>
       <c r="L26">
-        <v>0.9827856025039124</v>
+        <v>0.9930666666666667</v>
       </c>
       <c r="M26">
         <v>13976</v>
@@ -2124,7 +2127,7 @@
         <v>13976</v>
       </c>
       <c r="R26">
-        <v>95.58779336004579</v>
+        <v>124.8941041785919</v>
       </c>
       <c r="S26">
         <v>13976</v>
@@ -2132,7 +2135,7 @@
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
@@ -2150,43 +2153,43 @@
         <v>2E-05</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H27">
-        <v>0.9620394955194159</v>
+        <v>0.9968749313981738</v>
       </c>
       <c r="I27">
-        <v>0.7083333333333333</v>
+        <v>0.9823813321094111</v>
       </c>
       <c r="J27" t="s">
         <v>64</v>
       </c>
       <c r="K27">
-        <v>0.6666666666666666</v>
+        <v>0.9819770617149098</v>
       </c>
       <c r="L27">
-        <v>0.75</v>
+        <v>0.9827856025039124</v>
       </c>
       <c r="M27">
-        <v>915</v>
+        <v>13976</v>
       </c>
       <c r="N27">
-        <v>0.5715846994535519</v>
+        <v>0.5</v>
       </c>
       <c r="O27">
-        <v>1.167091836734694</v>
+        <v>1.00899723162104</v>
       </c>
       <c r="P27">
-        <v>0.8747609942638623</v>
+        <v>0.9911618069194742</v>
       </c>
       <c r="Q27">
-        <v>784</v>
+        <v>13976</v>
       </c>
       <c r="R27">
-        <v>23.13879781420765</v>
+        <v>95.58779336004579</v>
       </c>
       <c r="S27">
-        <v>915</v>
+        <v>13976</v>
       </c>
     </row>
     <row r="28" spans="1:19">
@@ -2197,34 +2200,34 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28">
         <v>256</v>
       </c>
       <c r="E28">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F28">
         <v>2E-05</v>
       </c>
       <c r="G28">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H28">
-        <v>0.9844451244390044</v>
+        <v>0.9988845884253192</v>
       </c>
       <c r="I28">
-        <v>0.8558352402745996</v>
+        <v>0.7980769230769231</v>
       </c>
       <c r="J28" t="s">
         <v>65</v>
       </c>
       <c r="K28">
-        <v>0.8421052631578948</v>
+        <v>0.75</v>
       </c>
       <c r="L28">
-        <v>0.8695652173913043</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="M28">
         <v>915</v>
@@ -2242,7 +2245,7 @@
         <v>784</v>
       </c>
       <c r="R28">
-        <v>18.76612021857924</v>
+        <v>23.13879781420765</v>
       </c>
       <c r="S28">
         <v>915</v>
@@ -2250,66 +2253,66 @@
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D29">
         <v>256</v>
       </c>
       <c r="E29">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F29">
         <v>2E-05</v>
       </c>
       <c r="G29">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H29">
-        <v>0.9698823662863867</v>
+        <v>0.9652841097543512</v>
       </c>
       <c r="I29">
-        <v>0.7827100228213903</v>
+        <v>0.8990384615384616</v>
       </c>
       <c r="J29" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="K29">
-        <v>0.6342141863699583</v>
+        <v>0.8750000000000001</v>
       </c>
       <c r="L29">
-        <v>0.9312058592728224</v>
+        <v>0.923076923076923</v>
       </c>
       <c r="M29">
-        <v>35841</v>
+        <v>915</v>
       </c>
       <c r="N29">
-        <v>0.8408526547808376</v>
+        <v>0.5715846994535519</v>
       </c>
       <c r="O29">
-        <v>3.108457711442786</v>
+        <v>1.167091836734694</v>
       </c>
       <c r="P29">
-        <v>0.5958420751478162</v>
+        <v>0.8747609942638623</v>
       </c>
       <c r="Q29">
-        <v>11408</v>
+        <v>784</v>
       </c>
       <c r="R29">
-        <v>138.1349571719539</v>
+        <v>18.76612021857924</v>
       </c>
       <c r="S29">
-        <v>35841</v>
+        <v>915</v>
       </c>
     </row>
     <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
@@ -2318,57 +2321,57 @@
         <v>38</v>
       </c>
       <c r="D30">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E30">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F30">
         <v>2E-05</v>
       </c>
       <c r="G30">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H30">
-        <v>0.9976842317049708</v>
+        <v>0.961995316274626</v>
       </c>
       <c r="I30">
-        <v>0.9377116809697217</v>
+        <v>0.824890017118312</v>
       </c>
       <c r="J30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K30">
-        <v>0.9128065395095368</v>
+        <v>0.7086383601756954</v>
       </c>
       <c r="L30">
-        <v>0.9626168224299065</v>
+        <v>0.9411416740609287</v>
       </c>
       <c r="M30">
-        <v>8702</v>
+        <v>35841</v>
       </c>
       <c r="N30">
-        <v>0.6836359457595955</v>
+        <v>0.8408526547808376</v>
       </c>
       <c r="O30">
-        <v>1.623955960516325</v>
+        <v>3.108457711442786</v>
       </c>
       <c r="P30">
-        <v>0.7224286438101672</v>
+        <v>0.5958420751478162</v>
       </c>
       <c r="Q30">
-        <v>5506</v>
+        <v>11408</v>
       </c>
       <c r="R30">
-        <v>41.82509767869455</v>
+        <v>110.2645015485059</v>
       </c>
       <c r="S30">
-        <v>8702</v>
+        <v>35841</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -2377,57 +2380,57 @@
         <v>37</v>
       </c>
       <c r="D31">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E31">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F31">
         <v>2E-05</v>
       </c>
       <c r="G31">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H31">
-        <v>0.9983554155560195</v>
+        <v>0.9936132868159206</v>
       </c>
       <c r="I31">
-        <v>0.9350975674953221</v>
+        <v>0.8047766186706919</v>
       </c>
       <c r="J31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K31">
-        <v>0.9069767441860466</v>
+        <v>0.6729452054794521</v>
       </c>
       <c r="L31">
-        <v>0.9632183908045977</v>
+        <v>0.9366080318619318</v>
       </c>
       <c r="M31">
-        <v>8702</v>
+        <v>35841</v>
       </c>
       <c r="N31">
-        <v>0.6836359457595955</v>
+        <v>0.8408526547808376</v>
       </c>
       <c r="O31">
-        <v>1.623955960516325</v>
+        <v>3.108457711442786</v>
       </c>
       <c r="P31">
-        <v>0.7224286438101672</v>
+        <v>0.5958420751478162</v>
       </c>
       <c r="Q31">
-        <v>5506</v>
+        <v>11408</v>
       </c>
       <c r="R31">
-        <v>47.90197655711331</v>
+        <v>138.1349571719539</v>
       </c>
       <c r="S31">
-        <v>8702</v>
+        <v>35841</v>
       </c>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -2445,48 +2448,48 @@
         <v>2E-05</v>
       </c>
       <c r="G32">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H32">
-        <v>0.9982256953292372</v>
+        <v>0.9976842317049708</v>
       </c>
       <c r="I32">
-        <v>0.8480383127647817</v>
+        <v>0.9377116809697217</v>
       </c>
       <c r="J32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K32">
-        <v>0.8764044943820225</v>
+        <v>0.9128065395095368</v>
       </c>
       <c r="L32">
-        <v>0.819672131147541</v>
+        <v>0.9626168224299065</v>
       </c>
       <c r="M32">
-        <v>564</v>
+        <v>8702</v>
       </c>
       <c r="N32">
-        <v>0.5141843971631206</v>
+        <v>0.6836359457595955</v>
       </c>
       <c r="O32">
-        <v>1.029197080291971</v>
+        <v>1.623955960516325</v>
       </c>
       <c r="P32">
-        <v>0.9724137931034482</v>
+        <v>0.7224286438101672</v>
       </c>
       <c r="Q32">
-        <v>548</v>
+        <v>5506</v>
       </c>
       <c r="R32">
-        <v>27.86170212765957</v>
+        <v>41.82509767869455</v>
       </c>
       <c r="S32">
-        <v>564</v>
+        <v>8702</v>
       </c>
     </row>
     <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
@@ -2504,160 +2507,278 @@
         <v>2E-05</v>
       </c>
       <c r="G33">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0.9983554155560195</v>
       </c>
       <c r="I33">
-        <v>0.8625366568914956</v>
+        <v>0.9350975674953221</v>
       </c>
       <c r="J33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K33">
-        <v>0.8863636363636365</v>
+        <v>0.9069767441860466</v>
       </c>
       <c r="L33">
-        <v>0.8387096774193549</v>
+        <v>0.9632183908045977</v>
       </c>
       <c r="M33">
-        <v>564</v>
+        <v>8702</v>
       </c>
       <c r="N33">
-        <v>0.5141843971631206</v>
+        <v>0.6836359457595955</v>
       </c>
       <c r="O33">
-        <v>1.029197080291971</v>
+        <v>1.623955960516325</v>
       </c>
       <c r="P33">
-        <v>0.9724137931034482</v>
+        <v>0.7224286438101672</v>
       </c>
       <c r="Q33">
-        <v>548</v>
+        <v>5506</v>
       </c>
       <c r="R33">
-        <v>32.26950354609929</v>
+        <v>47.90197655711331</v>
       </c>
       <c r="S33">
-        <v>564</v>
+        <v>8702</v>
       </c>
     </row>
     <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D34">
         <v>256</v>
       </c>
       <c r="E34">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F34">
         <v>2E-05</v>
       </c>
       <c r="G34">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H34">
-        <v>0.9977395024203535</v>
+        <v>0.9982253380196158</v>
       </c>
       <c r="I34">
-        <v>0.6302521008403361</v>
+        <v>0.8637354651162791</v>
       </c>
       <c r="J34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K34">
-        <v>0.7843137254901961</v>
+        <v>0.8837209302325582</v>
       </c>
       <c r="L34">
-        <v>0.4761904761904762</v>
+        <v>0.84375</v>
       </c>
       <c r="M34">
-        <v>502</v>
+        <v>564</v>
       </c>
       <c r="N34">
-        <v>0.3286852589641434</v>
+        <v>0.5141843971631206</v>
       </c>
       <c r="O34">
-        <v>0.744807121661721</v>
+        <v>1.029197080291971</v>
       </c>
       <c r="P34">
-        <v>1.521212121212121</v>
+        <v>0.9724137931034482</v>
       </c>
       <c r="Q34">
-        <v>330</v>
+        <v>548</v>
       </c>
       <c r="R34">
-        <v>51.05577689243028</v>
+        <v>27.86170212765957</v>
       </c>
       <c r="S34">
-        <v>502</v>
+        <v>564</v>
       </c>
     </row>
     <row r="35" spans="1:19">
       <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35">
+        <v>256</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <v>2E-05</v>
+      </c>
+      <c r="G35">
+        <v>10</v>
+      </c>
+      <c r="H35">
+        <v>0.9928988718775181</v>
+      </c>
+      <c r="I35">
+        <v>0.8637354651162791</v>
+      </c>
+      <c r="J35" t="s">
+        <v>71</v>
+      </c>
+      <c r="K35">
+        <v>0.8837209302325582</v>
+      </c>
+      <c r="L35">
+        <v>0.84375</v>
+      </c>
+      <c r="M35">
+        <v>564</v>
+      </c>
+      <c r="N35">
+        <v>0.5141843971631206</v>
+      </c>
+      <c r="O35">
+        <v>1.029197080291971</v>
+      </c>
+      <c r="P35">
+        <v>0.9724137931034482</v>
+      </c>
+      <c r="Q35">
+        <v>548</v>
+      </c>
+      <c r="R35">
+        <v>32.26950354609929</v>
+      </c>
+      <c r="S35">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B35" t="b">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B36" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36">
+        <v>256</v>
+      </c>
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="F36">
+        <v>2E-05</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
+      <c r="H36">
+        <v>0.8927570412906755</v>
+      </c>
+      <c r="I36">
+        <v>0.6785714285714286</v>
+      </c>
+      <c r="J36" t="s">
+        <v>72</v>
+      </c>
+      <c r="K36">
+        <v>0.75</v>
+      </c>
+      <c r="L36">
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="M36">
+        <v>502</v>
+      </c>
+      <c r="N36">
+        <v>0.3286852589641434</v>
+      </c>
+      <c r="O36">
+        <v>0.744807121661721</v>
+      </c>
+      <c r="P36">
+        <v>1.521212121212121</v>
+      </c>
+      <c r="Q36">
+        <v>330</v>
+      </c>
+      <c r="R36">
+        <v>51.05577689243028</v>
+      </c>
+      <c r="S36">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
         <v>38</v>
       </c>
-      <c r="D35">
-        <v>256</v>
-      </c>
-      <c r="E35">
+      <c r="D37">
+        <v>256</v>
+      </c>
+      <c r="E37">
         <v>16</v>
       </c>
-      <c r="F35">
-        <v>2E-05</v>
-      </c>
-      <c r="G35">
+      <c r="F37">
+        <v>2E-05</v>
+      </c>
+      <c r="G37">
         <v>27</v>
       </c>
-      <c r="H35">
+      <c r="H37">
         <v>0.9329232612251481</v>
       </c>
-      <c r="I35">
+      <c r="I37">
         <v>0.6544581965142713</v>
       </c>
-      <c r="J35" t="s">
-        <v>72</v>
-      </c>
-      <c r="K35">
+      <c r="J37" t="s">
+        <v>73</v>
+      </c>
+      <c r="K37">
         <v>0.8224299065420561</v>
       </c>
-      <c r="L35">
+      <c r="L37">
         <v>0.4864864864864865</v>
       </c>
-      <c r="M35">
+      <c r="M37">
         <v>502</v>
       </c>
-      <c r="N35">
+      <c r="N37">
         <v>0.3286852589641434</v>
       </c>
-      <c r="O35">
+      <c r="O37">
         <v>0.744807121661721</v>
       </c>
-      <c r="P35">
+      <c r="P37">
         <v>1.521212121212121</v>
       </c>
-      <c r="Q35">
+      <c r="Q37">
         <v>330</v>
       </c>
-      <c r="R35">
+      <c r="R37">
         <v>50.84262948207171</v>
       </c>
-      <c r="S35">
+      <c r="S37">
         <v>502</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated training summary for sentiment
</commit_message>
<xml_diff>
--- a/fine_tuning/training_summary_acl_sentiment.xlsx
+++ b/fine_tuning/training_summary_acl_sentiment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="78">
   <si>
     <t>training_lang</t>
   </si>
@@ -100,6 +100,9 @@
     <t>Cantonese</t>
   </si>
   <si>
+    <t>Indonesian</t>
+  </si>
+  <si>
     <t>Finnish</t>
   </si>
   <si>
@@ -157,10 +160,10 @@
     <t>0:07:58</t>
   </si>
   <si>
-    <t>0:12:08</t>
-  </si>
-  <si>
-    <t>0:12:09</t>
+    <t>0:41:56</t>
+  </si>
+  <si>
+    <t>0:16:01</t>
   </si>
   <si>
     <t>2:41:02</t>
@@ -187,37 +190,46 @@
     <t>4:04:22</t>
   </si>
   <si>
-    <t>0:20:22</t>
-  </si>
-  <si>
-    <t>0:34:10</t>
+    <t>0:52:22</t>
+  </si>
+  <si>
+    <t>0:53:17</t>
+  </si>
+  <si>
+    <t>0:34:13</t>
+  </si>
+  <si>
+    <t>0:29:01</t>
+  </si>
+  <si>
+    <t>0:52:43</t>
   </si>
   <si>
     <t>0:19:15</t>
   </si>
   <si>
-    <t>0:52:43</t>
-  </si>
-  <si>
-    <t>0:14:52</t>
-  </si>
-  <si>
-    <t>0:32:51</t>
+    <t>1:52:33</t>
+  </si>
+  <si>
+    <t>7:58:09</t>
+  </si>
+  <si>
+    <t>1:25:08</t>
   </si>
   <si>
     <t>2:01:23</t>
   </si>
   <si>
-    <t>1:25:08</t>
-  </si>
-  <si>
-    <t>0:21:10</t>
-  </si>
-  <si>
-    <t>4:18:45</t>
-  </si>
-  <si>
-    <t>2:14:46</t>
+    <t>0:50:35</t>
+  </si>
+  <si>
+    <t>2:14:12</t>
+  </si>
+  <si>
+    <t>0:07:05</t>
+  </si>
+  <si>
+    <t>0:16:30</t>
   </si>
   <si>
     <t>2:23:47</t>
@@ -593,7 +605,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -666,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>256</v>
@@ -687,7 +699,7 @@
         <v>0.8385384949978252</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K2">
         <v>0.7603305785123967</v>
@@ -725,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3">
         <v>256</v>
@@ -746,7 +758,7 @@
         <v>0.8600632462084543</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K3">
         <v>0.7946666666666667</v>
@@ -784,7 +796,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>256</v>
@@ -805,7 +817,7 @@
         <v>0.8638888888888889</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K4">
         <v>0.7777777777777779</v>
@@ -843,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D5">
         <v>256</v>
@@ -864,7 +876,7 @@
         <v>0.9654740468175057</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K5">
         <v>0.9433962264150944</v>
@@ -902,7 +914,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>256</v>
@@ -923,7 +935,7 @@
         <v>0.9522076810176126</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K6">
         <v>0.9178082191780821</v>
@@ -961,7 +973,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>256</v>
@@ -982,7 +994,7 @@
         <v>0.9371932107161867</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K7">
         <v>0.8918918918918919</v>
@@ -1020,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>256</v>
@@ -1041,7 +1053,7 @@
         <v>0.729086055899936</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K8">
         <v>0.6246056782334385</v>
@@ -1079,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>256</v>
@@ -1100,7 +1112,7 @@
         <v>0.8284664508791881</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K9">
         <v>0.7639751552795031</v>
@@ -1138,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>256</v>
@@ -1150,22 +1162,22 @@
         <v>2E-05</v>
       </c>
       <c r="G10">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0.9946393839875012</v>
       </c>
       <c r="I10">
-        <v>0.9288793103448276</v>
+        <v>0.8816111809045226</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K10">
-        <v>0.9827586206896551</v>
+        <v>0.8944723618090452</v>
       </c>
       <c r="L10">
-        <v>0.875</v>
+        <v>0.86875</v>
       </c>
       <c r="M10">
         <v>462</v>
@@ -1197,34 +1209,34 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="E11">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F11">
-        <v>2E-06</v>
+        <v>2E-05</v>
       </c>
       <c r="G11">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="H11">
-        <v>0.969041769041769</v>
+        <v>0.9502462525329791</v>
       </c>
       <c r="I11">
-        <v>0.9200968523002421</v>
+        <v>0.9034763313609467</v>
       </c>
       <c r="J11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K11">
-        <v>0.9830508474576271</v>
+        <v>0.9134615384615384</v>
       </c>
       <c r="L11">
-        <v>0.8571428571428571</v>
+        <v>0.893491124260355</v>
       </c>
       <c r="M11">
         <v>462</v>
@@ -1256,7 +1268,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>256</v>
@@ -1277,7 +1289,7 @@
         <v>0.9619984492699006</v>
       </c>
       <c r="J12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K12">
         <v>0.9544787077826725</v>
@@ -1315,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13">
         <v>256</v>
@@ -1336,7 +1348,7 @@
         <v>0.9639206342202415</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K13">
         <v>0.9567430025445293</v>
@@ -1374,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14">
         <v>256</v>
@@ -1395,7 +1407,7 @@
         <v>0.9082603020697371</v>
       </c>
       <c r="J14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K14">
         <v>0.9132947976878614</v>
@@ -1433,7 +1445,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>256</v>
@@ -1454,7 +1466,7 @@
         <v>0.8533914403844005</v>
       </c>
       <c r="J15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K15">
         <v>0.8596491228070176</v>
@@ -1492,7 +1504,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D16">
         <v>256</v>
@@ -1513,7 +1525,7 @@
         <v>0.9021451718722042</v>
       </c>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K16">
         <v>0.9238434163701068</v>
@@ -1551,7 +1563,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D17">
         <v>256</v>
@@ -1572,7 +1584,7 @@
         <v>0.8383446776656489</v>
       </c>
       <c r="J17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K17">
         <v>0.8672168042010502</v>
@@ -1610,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D18">
         <v>256</v>
@@ -1631,7 +1643,7 @@
         <v>0.925558022671497</v>
       </c>
       <c r="J18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K18">
         <v>0.8743718592964823</v>
@@ -1669,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19">
         <v>256</v>
@@ -1690,7 +1702,7 @@
         <v>0.9307842026806231</v>
       </c>
       <c r="J19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K19">
         <v>0.881949733434882</v>
@@ -1728,55 +1740,55 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>256</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F20">
         <v>2E-05</v>
       </c>
       <c r="G20">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H20">
-        <v>0.9951478755388181</v>
+        <v>0.9911926727837921</v>
       </c>
       <c r="I20">
-        <v>0.8207885304659498</v>
+        <v>0.9388089280085956</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K20">
-        <v>0.7311827956989247</v>
+        <v>0.9236192714453584</v>
       </c>
       <c r="L20">
-        <v>0.9103942652329748</v>
+        <v>0.953998584571833</v>
       </c>
       <c r="M20">
-        <v>1355</v>
+        <v>11881</v>
       </c>
       <c r="N20">
-        <v>0.7158671586715867</v>
+        <v>0.7602053699183571</v>
       </c>
       <c r="O20">
-        <v>1.789325842696629</v>
+        <v>7.620301323999391</v>
       </c>
       <c r="P20">
-        <v>0.6938997821350763</v>
+        <v>0.5351108736307775</v>
       </c>
       <c r="Q20">
-        <v>770</v>
+        <v>5698</v>
       </c>
       <c r="R20">
-        <v>93.26125461254613</v>
+        <v>23.65002945879976</v>
       </c>
       <c r="S20">
-        <v>1355</v>
+        <v>11881</v>
       </c>
     </row>
     <row r="21" spans="1:19">
@@ -1787,55 +1799,55 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D21">
         <v>256</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F21">
         <v>2E-05</v>
       </c>
       <c r="G21">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0.9936421583306182</v>
       </c>
       <c r="I21">
-        <v>0.9433623014683847</v>
+        <v>0.9604392494606553</v>
       </c>
       <c r="J21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K21">
-        <v>0.9148936170212766</v>
+        <v>0.9489414694894146</v>
       </c>
       <c r="L21">
-        <v>0.971830985915493</v>
+        <v>0.9719370294318959</v>
       </c>
       <c r="M21">
-        <v>1355</v>
+        <v>11881</v>
       </c>
       <c r="N21">
-        <v>0.7158671586715867</v>
+        <v>0.7602053699183571</v>
       </c>
       <c r="O21">
-        <v>1.789325842696629</v>
+        <v>7.620301323999391</v>
       </c>
       <c r="P21">
-        <v>0.6938997821350763</v>
+        <v>0.5351108736307775</v>
       </c>
       <c r="Q21">
-        <v>770</v>
+        <v>5698</v>
       </c>
       <c r="R21">
-        <v>80.20959409594096</v>
+        <v>19.45181382038549</v>
       </c>
       <c r="S21">
-        <v>1355</v>
+        <v>11881</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -1846,55 +1858,55 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D22">
         <v>256</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F22">
         <v>2E-05</v>
       </c>
       <c r="G22">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0.9981487137142231</v>
       </c>
       <c r="I22">
-        <v>0.8907860824742269</v>
+        <v>0.9317670042671328</v>
       </c>
       <c r="J22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K22">
-        <v>0.8125</v>
+        <v>0.9427792915531336</v>
       </c>
       <c r="L22">
-        <v>0.9690721649484536</v>
+        <v>0.920754716981132</v>
       </c>
       <c r="M22">
-        <v>789</v>
+        <v>1355</v>
       </c>
       <c r="N22">
-        <v>0.8466413181242078</v>
+        <v>0.7158671586715867</v>
       </c>
       <c r="O22">
-        <v>3.260330578512397</v>
+        <v>1.789325842696629</v>
       </c>
       <c r="P22">
-        <v>0.5905688622754491</v>
+        <v>0.6938997821350763</v>
       </c>
       <c r="Q22">
-        <v>242</v>
+        <v>770</v>
       </c>
       <c r="R22">
-        <v>21.44993662864385</v>
+        <v>80.20959409594096</v>
       </c>
       <c r="S22">
-        <v>789</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -1917,43 +1929,43 @@
         <v>2E-05</v>
       </c>
       <c r="G23">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="H23">
-        <v>0.9975678549960697</v>
+        <v>0.9983792461311243</v>
       </c>
       <c r="I23">
-        <v>0.9112890563667766</v>
+        <v>0.8904863508812766</v>
       </c>
       <c r="J23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K23">
-        <v>0.8484848484848485</v>
+        <v>0.9100671140939597</v>
       </c>
       <c r="L23">
-        <v>0.9740932642487047</v>
+        <v>0.8709055876685934</v>
       </c>
       <c r="M23">
-        <v>789</v>
+        <v>1355</v>
       </c>
       <c r="N23">
-        <v>0.8466413181242078</v>
+        <v>0.7158671586715867</v>
       </c>
       <c r="O23">
-        <v>3.260330578512397</v>
+        <v>1.789325842696629</v>
       </c>
       <c r="P23">
-        <v>0.5905688622754491</v>
+        <v>0.6938997821350763</v>
       </c>
       <c r="Q23">
-        <v>242</v>
+        <v>770</v>
       </c>
       <c r="R23">
-        <v>19.80481622306717</v>
+        <v>93.26125461254613</v>
       </c>
       <c r="S23">
-        <v>789</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -1964,55 +1976,55 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D24">
         <v>256</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F24">
         <v>2E-05</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="H24">
-        <v>0.9555193039907464</v>
+        <v>0.9975678549960697</v>
       </c>
       <c r="I24">
-        <v>0.7485134362492853</v>
+        <v>0.9112890563667766</v>
       </c>
       <c r="J24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K24">
-        <v>0.712121212121212</v>
+        <v>0.8484848484848485</v>
       </c>
       <c r="L24">
-        <v>0.7849056603773585</v>
+        <v>0.9740932642487047</v>
       </c>
       <c r="M24">
-        <v>3237</v>
+        <v>789</v>
       </c>
       <c r="N24">
-        <v>0.5817114612295335</v>
+        <v>0.8466413181242078</v>
       </c>
       <c r="O24">
-        <v>1.195347119645495</v>
+        <v>3.260330578512397</v>
       </c>
       <c r="P24">
-        <v>0.8595326606479022</v>
+        <v>0.5905688622754491</v>
       </c>
       <c r="Q24">
-        <v>2708</v>
+        <v>242</v>
       </c>
       <c r="R24">
-        <v>44.17763361136855</v>
+        <v>19.80481622306717</v>
       </c>
       <c r="S24">
-        <v>3237</v>
+        <v>789</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -2035,43 +2047,43 @@
         <v>2E-05</v>
       </c>
       <c r="G25">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H25">
-        <v>0.9886034057168788</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>0.8188714171214839</v>
+        <v>0.8907860824742269</v>
       </c>
       <c r="J25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K25">
-        <v>0.7918781725888325</v>
+        <v>0.8125</v>
       </c>
       <c r="L25">
-        <v>0.8458646616541353</v>
+        <v>0.9690721649484536</v>
       </c>
       <c r="M25">
-        <v>3237</v>
+        <v>789</v>
       </c>
       <c r="N25">
-        <v>0.5817114612295335</v>
+        <v>0.8466413181242078</v>
       </c>
       <c r="O25">
-        <v>1.195347119645495</v>
+        <v>3.260330578512397</v>
       </c>
       <c r="P25">
-        <v>0.8595326606479022</v>
+        <v>0.5905688622754491</v>
       </c>
       <c r="Q25">
-        <v>2708</v>
+        <v>242</v>
       </c>
       <c r="R25">
-        <v>39.5863453815261</v>
+        <v>21.44993662864385</v>
       </c>
       <c r="S25">
-        <v>3237</v>
+        <v>789</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -2094,43 +2106,43 @@
         <v>2E-05</v>
       </c>
       <c r="G26">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H26">
-        <v>0.9970701290812722</v>
+        <v>0.9434937701881632</v>
       </c>
       <c r="I26">
-        <v>0.9875182577465661</v>
+        <v>0.8481845244807289</v>
       </c>
       <c r="J26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K26">
-        <v>0.9846416382252561</v>
+        <v>0.841692789968652</v>
       </c>
       <c r="L26">
-        <v>0.9903948772678761</v>
+        <v>0.8546762589928057</v>
       </c>
       <c r="M26">
-        <v>9831</v>
+        <v>3237</v>
       </c>
       <c r="N26">
-        <v>0.6184518360288882</v>
+        <v>0.5817114612295335</v>
       </c>
       <c r="O26">
-        <v>1.00899723162104</v>
+        <v>1.195347119645495</v>
       </c>
       <c r="P26">
-        <v>0.9911618069194742</v>
+        <v>0.8595326606479022</v>
       </c>
       <c r="Q26">
-        <v>7502</v>
+        <v>2708</v>
       </c>
       <c r="R26">
-        <v>125.2016071610213</v>
+        <v>44.17763361136855</v>
       </c>
       <c r="S26">
-        <v>9831</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="27" spans="1:19">
@@ -2141,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D27">
         <v>256</v>
@@ -2153,43 +2165,43 @@
         <v>2E-05</v>
       </c>
       <c r="G27">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H27">
-        <v>0.9964145768862624</v>
+        <v>0.9938993274008461</v>
       </c>
       <c r="I27">
-        <v>0.9827719455890884</v>
+        <v>0.8813688204361012</v>
       </c>
       <c r="J27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K27">
-        <v>0.9790996784565917</v>
+        <v>0.8778979907264296</v>
       </c>
       <c r="L27">
-        <v>0.986444212721585</v>
+        <v>0.8848396501457727</v>
       </c>
       <c r="M27">
-        <v>9831</v>
+        <v>3237</v>
       </c>
       <c r="N27">
-        <v>0.6184518360288882</v>
+        <v>0.5817114612295335</v>
       </c>
       <c r="O27">
-        <v>1.00899723162104</v>
+        <v>1.195347119645495</v>
       </c>
       <c r="P27">
-        <v>0.9911618069194742</v>
+        <v>0.8595326606479022</v>
       </c>
       <c r="Q27">
-        <v>7502</v>
+        <v>2708</v>
       </c>
       <c r="R27">
-        <v>96.22693520496389</v>
+        <v>39.5863453815261</v>
       </c>
       <c r="S27">
-        <v>9831</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="28" spans="1:19">
@@ -2200,55 +2212,55 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D28">
         <v>256</v>
       </c>
       <c r="E28">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F28">
         <v>2E-05</v>
       </c>
       <c r="G28">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H28">
-        <v>0.9988845884253192</v>
+        <v>0.9964145768862624</v>
       </c>
       <c r="I28">
-        <v>0.7980769230769231</v>
+        <v>0.9827719455890884</v>
       </c>
       <c r="J28" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K28">
-        <v>0.75</v>
+        <v>0.9790996784565917</v>
       </c>
       <c r="L28">
-        <v>0.8461538461538461</v>
+        <v>0.986444212721585</v>
       </c>
       <c r="M28">
-        <v>915</v>
+        <v>9831</v>
       </c>
       <c r="N28">
-        <v>0.5715846994535519</v>
+        <v>0.6184518360288882</v>
       </c>
       <c r="O28">
-        <v>1.167091836734694</v>
+        <v>1.00899723162104</v>
       </c>
       <c r="P28">
-        <v>0.8747609942638623</v>
+        <v>0.9911618069194742</v>
       </c>
       <c r="Q28">
-        <v>784</v>
+        <v>7502</v>
       </c>
       <c r="R28">
-        <v>23.13879781420765</v>
+        <v>96.22693520496389</v>
       </c>
       <c r="S28">
-        <v>915</v>
+        <v>9831</v>
       </c>
     </row>
     <row r="29" spans="1:19">
@@ -2259,55 +2271,55 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D29">
         <v>256</v>
       </c>
       <c r="E29">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F29">
         <v>2E-05</v>
       </c>
       <c r="G29">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H29">
-        <v>0.9652841097543512</v>
+        <v>0.9970701290812722</v>
       </c>
       <c r="I29">
-        <v>0.8990384615384616</v>
+        <v>0.9875182577465661</v>
       </c>
       <c r="J29" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="K29">
-        <v>0.8750000000000001</v>
+        <v>0.9846416382252561</v>
       </c>
       <c r="L29">
-        <v>0.923076923076923</v>
+        <v>0.9903948772678761</v>
       </c>
       <c r="M29">
-        <v>915</v>
+        <v>9831</v>
       </c>
       <c r="N29">
-        <v>0.5715846994535519</v>
+        <v>0.6184518360288882</v>
       </c>
       <c r="O29">
-        <v>1.167091836734694</v>
+        <v>1.00899723162104</v>
       </c>
       <c r="P29">
-        <v>0.8747609942638623</v>
+        <v>0.9911618069194742</v>
       </c>
       <c r="Q29">
-        <v>784</v>
+        <v>7502</v>
       </c>
       <c r="R29">
-        <v>18.76612021857924</v>
+        <v>125.2016071610213</v>
       </c>
       <c r="S29">
-        <v>915</v>
+        <v>9831</v>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -2321,52 +2333,52 @@
         <v>38</v>
       </c>
       <c r="D30">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="E30">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F30">
         <v>2E-05</v>
       </c>
       <c r="G30">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="H30">
-        <v>0.9985252995190412</v>
+        <v>0.9968471305696303</v>
       </c>
       <c r="I30">
-        <v>0.8366805134655178</v>
+        <v>0.8570910080754921</v>
       </c>
       <c r="J30" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K30">
-        <v>0.7248979591836734</v>
+        <v>0.8543689320388349</v>
       </c>
       <c r="L30">
-        <v>0.9484630677473621</v>
+        <v>0.8598130841121494</v>
       </c>
       <c r="M30">
-        <v>33976</v>
+        <v>915</v>
       </c>
       <c r="N30">
-        <v>0.8393571933129268</v>
+        <v>0.5715846994535519</v>
       </c>
       <c r="O30">
-        <v>3.108457711442786</v>
+        <v>1.167091836734694</v>
       </c>
       <c r="P30">
-        <v>0.5958420751478162</v>
+        <v>0.8747609942638623</v>
       </c>
       <c r="Q30">
-        <v>10916</v>
+        <v>784</v>
       </c>
       <c r="R30">
-        <v>114.1969036967271</v>
+        <v>23.13879781420765</v>
       </c>
       <c r="S30">
-        <v>33976</v>
+        <v>915</v>
       </c>
     </row>
     <row r="31" spans="1:19">
@@ -2377,55 +2389,55 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D31">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="E31">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F31">
         <v>2E-05</v>
       </c>
       <c r="G31">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H31">
-        <v>0.9936132868159206</v>
+        <v>0.9984347216427809</v>
       </c>
       <c r="I31">
-        <v>0.8047766186706919</v>
+        <v>0.9142857142857144</v>
       </c>
       <c r="J31" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K31">
-        <v>0.6729452054794521</v>
+        <v>0.9142857142857144</v>
       </c>
       <c r="L31">
-        <v>0.9366080318619318</v>
+        <v>0.9142857142857144</v>
       </c>
       <c r="M31">
-        <v>33976</v>
+        <v>915</v>
       </c>
       <c r="N31">
-        <v>0.8393571933129268</v>
+        <v>0.5715846994535519</v>
       </c>
       <c r="O31">
-        <v>3.108457711442786</v>
+        <v>1.167091836734694</v>
       </c>
       <c r="P31">
-        <v>0.5958420751478162</v>
+        <v>0.8747609942638623</v>
       </c>
       <c r="Q31">
-        <v>10916</v>
+        <v>784</v>
       </c>
       <c r="R31">
-        <v>143.0427360489757</v>
+        <v>18.76612021857924</v>
       </c>
       <c r="S31">
-        <v>33976</v>
+        <v>915</v>
       </c>
     </row>
     <row r="32" spans="1:19">
@@ -2436,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D32">
         <v>256</v>
@@ -2448,43 +2460,43 @@
         <v>2E-05</v>
       </c>
       <c r="G32">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="H32">
-        <v>0.9976842317049708</v>
+        <v>0.9134590042638803</v>
       </c>
       <c r="I32">
-        <v>0.9377116809697217</v>
+        <v>0.8945204926307289</v>
       </c>
       <c r="J32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K32">
-        <v>0.9128065395095368</v>
+        <v>0.9028871391076114</v>
       </c>
       <c r="L32">
-        <v>0.9626168224299065</v>
+        <v>0.8861538461538462</v>
       </c>
       <c r="M32">
-        <v>6621</v>
+        <v>33976</v>
       </c>
       <c r="N32">
-        <v>0.7066908322005739</v>
+        <v>0.8393571933129268</v>
       </c>
       <c r="O32">
-        <v>1.623955960516325</v>
+        <v>3.108457711442786</v>
       </c>
       <c r="P32">
-        <v>0.7224286438101672</v>
+        <v>0.5958420751478162</v>
       </c>
       <c r="Q32">
-        <v>3884</v>
+        <v>10916</v>
       </c>
       <c r="R32">
-        <v>40.97130342848512</v>
+        <v>114.1969036967271</v>
       </c>
       <c r="S32">
-        <v>6621</v>
+        <v>33976</v>
       </c>
     </row>
     <row r="33" spans="1:19">
@@ -2495,7 +2507,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D33">
         <v>256</v>
@@ -2507,43 +2519,43 @@
         <v>2E-05</v>
       </c>
       <c r="G33">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H33">
-        <v>0.9994357827839917</v>
+        <v>0.9967474837622093</v>
       </c>
       <c r="I33">
-        <v>0.9359135083000885</v>
+        <v>0.8835499054592268</v>
       </c>
       <c r="J33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K33">
-        <v>0.9088191330343797</v>
+        <v>0.8894878706199462</v>
       </c>
       <c r="L33">
-        <v>0.9630078835657974</v>
+        <v>0.8776119402985074</v>
       </c>
       <c r="M33">
-        <v>6621</v>
+        <v>33976</v>
       </c>
       <c r="N33">
-        <v>0.7066908322005739</v>
+        <v>0.8393571933129268</v>
       </c>
       <c r="O33">
-        <v>1.623955960516325</v>
+        <v>3.108457711442786</v>
       </c>
       <c r="P33">
-        <v>0.7224286438101672</v>
+        <v>0.5958420751478162</v>
       </c>
       <c r="Q33">
-        <v>3884</v>
+        <v>10916</v>
       </c>
       <c r="R33">
-        <v>46.88385440265821</v>
+        <v>143.0427360489757</v>
       </c>
       <c r="S33">
-        <v>6621</v>
+        <v>33976</v>
       </c>
     </row>
     <row r="34" spans="1:19">
@@ -2554,55 +2566,55 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D34">
         <v>256</v>
       </c>
       <c r="E34">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F34">
         <v>2E-05</v>
       </c>
       <c r="G34">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="H34">
-        <v>0.9982253380196158</v>
+        <v>0.9976842317049708</v>
       </c>
       <c r="I34">
-        <v>0.8637354651162791</v>
+        <v>0.9377116809697217</v>
       </c>
       <c r="J34" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K34">
-        <v>0.8837209302325582</v>
+        <v>0.9128065395095368</v>
       </c>
       <c r="L34">
-        <v>0.84375</v>
+        <v>0.9626168224299065</v>
       </c>
       <c r="M34">
-        <v>564</v>
+        <v>6621</v>
       </c>
       <c r="N34">
-        <v>0.5141843971631206</v>
+        <v>0.7066908322005739</v>
       </c>
       <c r="O34">
-        <v>1.029197080291971</v>
+        <v>1.623955960516325</v>
       </c>
       <c r="P34">
-        <v>0.9724137931034482</v>
+        <v>0.7224286438101672</v>
       </c>
       <c r="Q34">
-        <v>548</v>
+        <v>3884</v>
       </c>
       <c r="R34">
-        <v>27.86170212765957</v>
+        <v>40.97130342848512</v>
       </c>
       <c r="S34">
-        <v>564</v>
+        <v>6621</v>
       </c>
     </row>
     <row r="35" spans="1:19">
@@ -2613,55 +2625,55 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D35">
         <v>256</v>
       </c>
       <c r="E35">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F35">
         <v>2E-05</v>
       </c>
       <c r="G35">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="H35">
-        <v>0.9928988718775181</v>
+        <v>0.9994357827839917</v>
       </c>
       <c r="I35">
-        <v>0.8637354651162791</v>
+        <v>0.9359135083000885</v>
       </c>
       <c r="J35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K35">
-        <v>0.8837209302325582</v>
+        <v>0.9088191330343797</v>
       </c>
       <c r="L35">
-        <v>0.84375</v>
+        <v>0.9630078835657974</v>
       </c>
       <c r="M35">
-        <v>564</v>
+        <v>6621</v>
       </c>
       <c r="N35">
-        <v>0.5141843971631206</v>
+        <v>0.7066908322005739</v>
       </c>
       <c r="O35">
-        <v>1.029197080291971</v>
+        <v>1.623955960516325</v>
       </c>
       <c r="P35">
-        <v>0.9724137931034482</v>
+        <v>0.7224286438101672</v>
       </c>
       <c r="Q35">
-        <v>548</v>
+        <v>3884</v>
       </c>
       <c r="R35">
-        <v>32.26950354609929</v>
+        <v>46.88385440265821</v>
       </c>
       <c r="S35">
-        <v>564</v>
+        <v>6621</v>
       </c>
     </row>
     <row r="36" spans="1:19">
@@ -2672,7 +2684,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D36">
         <v>256</v>
@@ -2684,43 +2696,43 @@
         <v>2E-05</v>
       </c>
       <c r="G36">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="H36">
-        <v>0.8927570412906755</v>
+        <v>0.9982253380196158</v>
       </c>
       <c r="I36">
-        <v>0.6785714285714286</v>
+        <v>0.8637354651162791</v>
       </c>
       <c r="J36" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K36">
-        <v>0.75</v>
+        <v>0.8837209302325582</v>
       </c>
       <c r="L36">
-        <v>0.6071428571428571</v>
+        <v>0.84375</v>
       </c>
       <c r="M36">
-        <v>502</v>
+        <v>564</v>
       </c>
       <c r="N36">
-        <v>0.3286852589641434</v>
+        <v>0.5141843971631206</v>
       </c>
       <c r="O36">
-        <v>0.744807121661721</v>
+        <v>1.029197080291971</v>
       </c>
       <c r="P36">
-        <v>1.521212121212121</v>
+        <v>0.9724137931034482</v>
       </c>
       <c r="Q36">
-        <v>330</v>
+        <v>548</v>
       </c>
       <c r="R36">
-        <v>51.05577689243028</v>
+        <v>27.86170212765957</v>
       </c>
       <c r="S36">
-        <v>502</v>
+        <v>564</v>
       </c>
     </row>
     <row r="37" spans="1:19">
@@ -2737,48 +2749,166 @@
         <v>256</v>
       </c>
       <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="F37">
+        <v>2E-05</v>
+      </c>
+      <c r="G37">
+        <v>10</v>
+      </c>
+      <c r="H37">
+        <v>0.9928988718775181</v>
+      </c>
+      <c r="I37">
+        <v>0.8637354651162791</v>
+      </c>
+      <c r="J37" t="s">
+        <v>75</v>
+      </c>
+      <c r="K37">
+        <v>0.8837209302325582</v>
+      </c>
+      <c r="L37">
+        <v>0.84375</v>
+      </c>
+      <c r="M37">
+        <v>564</v>
+      </c>
+      <c r="N37">
+        <v>0.5141843971631206</v>
+      </c>
+      <c r="O37">
+        <v>1.029197080291971</v>
+      </c>
+      <c r="P37">
+        <v>0.9724137931034482</v>
+      </c>
+      <c r="Q37">
+        <v>548</v>
+      </c>
+      <c r="R37">
+        <v>32.26950354609929</v>
+      </c>
+      <c r="S37">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38">
+        <v>256</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38">
+        <v>2E-05</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>0.8927570412906755</v>
+      </c>
+      <c r="I38">
+        <v>0.6785714285714286</v>
+      </c>
+      <c r="J38" t="s">
+        <v>76</v>
+      </c>
+      <c r="K38">
+        <v>0.75</v>
+      </c>
+      <c r="L38">
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="M38">
+        <v>502</v>
+      </c>
+      <c r="N38">
+        <v>0.3286852589641434</v>
+      </c>
+      <c r="O38">
+        <v>0.744807121661721</v>
+      </c>
+      <c r="P38">
+        <v>1.521212121212121</v>
+      </c>
+      <c r="Q38">
+        <v>330</v>
+      </c>
+      <c r="R38">
+        <v>51.05577689243028</v>
+      </c>
+      <c r="S38">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39">
+        <v>256</v>
+      </c>
+      <c r="E39">
         <v>16</v>
       </c>
-      <c r="F37">
-        <v>2E-05</v>
-      </c>
-      <c r="G37">
+      <c r="F39">
+        <v>2E-05</v>
+      </c>
+      <c r="G39">
         <v>27</v>
       </c>
-      <c r="H37">
+      <c r="H39">
         <v>0.9329232612251481</v>
       </c>
-      <c r="I37">
+      <c r="I39">
         <v>0.6544581965142713</v>
       </c>
-      <c r="J37" t="s">
-        <v>73</v>
-      </c>
-      <c r="K37">
+      <c r="J39" t="s">
+        <v>77</v>
+      </c>
+      <c r="K39">
         <v>0.8224299065420561</v>
       </c>
-      <c r="L37">
+      <c r="L39">
         <v>0.4864864864864865</v>
       </c>
-      <c r="M37">
+      <c r="M39">
         <v>502</v>
       </c>
-      <c r="N37">
+      <c r="N39">
         <v>0.3286852589641434</v>
       </c>
-      <c r="O37">
+      <c r="O39">
         <v>0.744807121661721</v>
       </c>
-      <c r="P37">
+      <c r="P39">
         <v>1.521212121212121</v>
       </c>
-      <c r="Q37">
+      <c r="Q39">
         <v>330</v>
       </c>
-      <c r="R37">
+      <c r="R39">
         <v>50.84262948207171</v>
       </c>
-      <c r="S37">
+      <c r="S39">
         <v>502</v>
       </c>
     </row>

</xml_diff>